<commit_message>
Adds B version and QA fixes
</commit_message>
<xml_diff>
--- a/knowledge-center/Error-Report.xlsx
+++ b/knowledge-center/Error-Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krono\OneDrive\Documents\GitHub\TDPrototype\knowledge-center\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8E57F4-16D5-4C3B-94A2-E163AE8CFBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA55605-9D7D-4944-9A13-645391A843A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42060" yWindow="5070" windowWidth="43920" windowHeight="23625" tabRatio="759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="6150" windowWidth="43920" windowHeight="23445" tabRatio="759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLE" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,12 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="SECTION 3" guid="{E4F6F464-F401-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="5"/>
+    <customWorkbookView name="SECTION 2" guid="{E4F6F463-F401-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="5"/>
+    <customWorkbookView name="MOE_SECTION1" guid="{485F31E0-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
+    <customWorkbookView name="MOE_SECTION2" guid="{485F31E1-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
+    <customWorkbookView name="MOE_SECTION3" guid="{485F31E2-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
     <customWorkbookView name="SECTION 1" guid="{B065B980-F71B-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="5"/>
-    <customWorkbookView name="MOE_SECTION3" guid="{485F31E2-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
-    <customWorkbookView name="MOE_SECTION2" guid="{485F31E1-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
-    <customWorkbookView name="MOE_SECTION1" guid="{485F31E0-F63A-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="16"/>
-    <customWorkbookView name="SECTION 2" guid="{E4F6F463-F401-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="5"/>
-    <customWorkbookView name="SECTION 3" guid="{E4F6F464-F401-11D2-A42E-006097D50F3E}" maximized="1" windowWidth="796" windowHeight="410" tabRatio="599" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -96,10 +96,10 @@
     <t>Social Security Number is not valid. Check that the SSN is 9 digits and enter 999999999 if individual does not have an SSN</t>
   </si>
   <si>
-    <t>Error</t>
+    <t>Error Description (3)</t>
   </si>
   <si>
-    <t xml:space="preserve">Exit date (YYYYMM) is not valid. </t>
+    <t>Exit date (YYYYMM) is not valid. Date must be in range of 2024-2025 Months 10-12</t>
   </si>
 </sst>
 </file>
@@ -220,14 +220,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
@@ -673,45 +673,45 @@
   </sheetPr>
   <dimension ref="A1:IA80"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="160" zoomScaleNormal="115" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A43" zoomScale="160" zoomScaleNormal="115" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:235" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:235" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -720,7 +720,7 @@
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -792,22 +792,22 @@
       <c r="A12" s="3">
         <v>202410</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>4788801898</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:235" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
@@ -1724,17 +1724,21 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="7">
+      <c r="A69" s="5">
         <v>202413</v>
       </c>
       <c r="B69" s="1">
         <v>272608410</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
@@ -1820,26 +1824,26 @@
       <c r="A80" s="3">
         <v>202412</v>
       </c>
-      <c r="B80" s="7">
+      <c r="B80" s="5">
         <v>520</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="7"/>
-      <c r="E80" s="7"/>
-      <c r="F80" s="7"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="7"/>
-      <c r="I80" s="7"/>
-      <c r="J80" s="7"/>
-      <c r="K80" s="7"/>
-      <c r="L80" s="7"/>
-      <c r="M80" s="7"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B065B980-F71B-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{E4F6F464-F401-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1849,7 +1853,7 @@
         <oddFooter>&amp;L&amp;F&amp;CPage &amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{485F31E2-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{E4F6F463-F401-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1859,7 +1863,7 @@
         <oddFooter>&amp;L&amp;F&amp;CPage &amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{485F31E1-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{485F31E0-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1869,7 +1873,7 @@
         <oddFooter>&amp;L&amp;F&amp;CPage &amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{485F31E0-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{485F31E1-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1879,7 +1883,7 @@
         <oddFooter>&amp;L&amp;F&amp;CPage &amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{E4F6F463-F401-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{485F31E2-F63A-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1889,7 +1893,7 @@
         <oddFooter>&amp;L&amp;F&amp;CPage &amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{E4F6F464-F401-11D2-A42E-006097D50F3E}" showRuler="0">
+    <customSheetView guid="{B065B980-F71B-11D2-A42E-006097D50F3E}" showRuler="0">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <printOptions gridLines="1"/>
@@ -1911,12 +1915,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2097,15 +2098,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{947173F8-8A53-4697-8B0E-D24B110213D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C49F0C-194B-446F-A859-45BEA59A7F08}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2130,10 +2135,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C49F0C-194B-446F-A859-45BEA59A7F08}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{947173F8-8A53-4697-8B0E-D24B110213D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>